<commit_message>
Report lacking 2 images
Everything is done except for a screenshot of keil executing the code,
and of the stack after corruption.
</commit_message>
<xml_diff>
--- a/Code Injection/gadgets.xlsx
+++ b/Code Injection/gadgets.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="92">
   <si>
     <t>Unexploited stack</t>
   </si>
@@ -135,6 +136,171 @@
   </si>
   <si>
     <t>// Return to 0x4BD8</t>
+  </si>
+  <si>
+    <t>0x400FD020</t>
+  </si>
+  <si>
+    <t>0xFFFFFFFF</t>
+  </si>
+  <si>
+    <t>0x400FD030</t>
+  </si>
+  <si>
+    <t>FLASH[0x30/4]=0xFFFFFFFF;</t>
+  </si>
+  <si>
+    <t>1b</t>
+  </si>
+  <si>
+    <t>Return to main</t>
+  </si>
+  <si>
+    <t>a14b 0000</t>
+  </si>
+  <si>
+    <t>0000 0000</t>
+  </si>
+  <si>
+    <t>Write flash key</t>
+  </si>
+  <si>
+    <t>7336 0000</t>
+  </si>
+  <si>
+    <t>20d0 0f40</t>
+  </si>
+  <si>
+    <t>Flash key</t>
+  </si>
+  <si>
+    <t>a742 0000</t>
+  </si>
+  <si>
+    <t>0100 42a4</t>
+  </si>
+  <si>
+    <t>Write clear</t>
+  </si>
+  <si>
+    <t>30d0 0f40</t>
+  </si>
+  <si>
+    <t>Clear write buffer</t>
+  </si>
+  <si>
+    <t>ffff ffff</t>
+  </si>
+  <si>
+    <t>Write b main</t>
+  </si>
+  <si>
+    <t>18d1 0f40</t>
+  </si>
+  <si>
+    <t>b main</t>
+  </si>
+  <si>
+    <t>42e0 0000</t>
+  </si>
+  <si>
+    <t>Write scatter addr</t>
+  </si>
+  <si>
+    <t>00d0 0f40</t>
+  </si>
+  <si>
+    <t>Scatter addr</t>
+  </si>
+  <si>
+    <t>584b 0000</t>
+  </si>
+  <si>
+    <t>Write b</t>
+  </si>
+  <si>
+    <t>24d1 0f40</t>
+  </si>
+  <si>
+    <t>fce7 5555</t>
+  </si>
+  <si>
+    <t>Write add</t>
+  </si>
+  <si>
+    <t>20d1 0f40</t>
+  </si>
+  <si>
+    <t>add R0,#0x1</t>
+  </si>
+  <si>
+    <t>00f1 0100</t>
+  </si>
+  <si>
+    <t>Write main address</t>
+  </si>
+  <si>
+    <t>main address</t>
+  </si>
+  <si>
+    <t>e04b 0000</t>
+  </si>
+  <si>
+    <t>Write erase command</t>
+  </si>
+  <si>
+    <t>08d0 0f40</t>
+  </si>
+  <si>
+    <t>Erase command</t>
+  </si>
+  <si>
+    <t>0200 42a4</t>
+  </si>
+  <si>
+    <t>Write erase address</t>
+  </si>
+  <si>
+    <t>Erase address</t>
+  </si>
+  <si>
+    <t>0048 0000</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>Return to A0</t>
+  </si>
+  <si>
+    <t>7536 0000</t>
+  </si>
+  <si>
+    <t>Fluff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000 0000 </t>
+  </si>
+  <si>
+    <t>3030 3030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3030 3030 </t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Pop into R4</t>
+  </si>
+  <si>
+    <t>Pop into PC</t>
+  </si>
+  <si>
+    <t>pop {pc}</t>
+  </si>
+  <si>
+    <t>Stack before attack</t>
   </si>
 </sst>
 </file>
@@ -178,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -192,6 +358,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,9 +787,6 @@
       <c r="K9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L9" s="2" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J10" s="2" t="s">
@@ -631,7 +795,9 @@
       <c r="K10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L10" s="2"/>
+      <c r="L10" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J11" s="2" t="s">
@@ -640,9 +806,6 @@
       <c r="K11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J12" s="2" t="s">
@@ -651,37 +814,484 @@
       <c r="K12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L12" s="2"/>
+      <c r="L12" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J15" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>